<commit_message>
update sok mono ve trifaz
</commit_message>
<xml_diff>
--- a/media/reports/TriFazSok.xlsx
+++ b/media/reports/TriFazSok.xlsx
@@ -19,8 +19,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt formatCode="0.000" numFmtId="164"/>
-    <numFmt formatCode="yyyy\-mm\-dd\ h:mm:ss" numFmtId="165"/>
+    <numFmt formatCode="yyyy\-mm\-dd\ h:mm:ss" numFmtId="164"/>
+    <numFmt formatCode="0.000" numFmtId="165"/>
   </numFmts>
   <fonts count="12">
     <font>
@@ -622,7 +622,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="102">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
@@ -746,45 +746,24 @@
     <xf applyAlignment="1" borderId="9" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="6" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="21" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="7" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="23" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="4" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="10" fillId="0" fontId="5" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf applyAlignment="1" borderId="13" fillId="0" fontId="5" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="13" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="5" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="20" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
     <xf applyAlignment="1" borderId="12" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
     <xf applyAlignment="1" borderId="3" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="18" fillId="0" fontId="5" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="3" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="18" fillId="0" fontId="5" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf borderId="4" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="10" fillId="0" fontId="5" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf applyAlignment="1" borderId="13" fillId="0" fontId="5" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="13" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="1" fillId="3" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -814,10 +793,40 @@
     <xf applyAlignment="1" borderId="20" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf applyAlignment="1" borderId="6" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="21" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="7" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="23" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="5" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="20" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf applyAlignment="1" borderId="25" fillId="6" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf applyAlignment="1" borderId="18" fillId="0" fontId="5" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="10" fillId="0" fontId="5" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
     <xf borderId="31" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="13" fillId="0" fontId="5" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
     <xf applyAlignment="1" borderId="16" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -1221,7 +1230,7 @@
   <dimension ref="A1:O46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -1249,17 +1258,17 @@
           <t>Trafo Tipi :</t>
         </is>
       </c>
-      <c r="B1" s="65" t="inlineStr">
+      <c r="B1" s="53" t="inlineStr">
         <is>
           <t xml:space="preserve"> Şok Trifaz Trafosu  Hesap Ozeti</t>
         </is>
       </c>
-      <c r="C1" s="58" t="n"/>
-      <c r="D1" s="58" t="n"/>
-      <c r="E1" s="58" t="n"/>
-      <c r="F1" s="58" t="n"/>
-      <c r="G1" s="58" t="n"/>
-      <c r="H1" s="58" t="n"/>
+      <c r="C1" s="55" t="n"/>
+      <c r="D1" s="55" t="n"/>
+      <c r="E1" s="55" t="n"/>
+      <c r="F1" s="55" t="n"/>
+      <c r="G1" s="55" t="n"/>
+      <c r="H1" s="55" t="n"/>
       <c r="I1" s="11" t="n"/>
       <c r="J1" s="6" t="inlineStr">
         <is>
@@ -1269,31 +1278,31 @@
       <c r="K1" s="27" t="n"/>
       <c r="L1" s="27" t="n"/>
       <c r="M1" s="27" t="n"/>
-      <c r="N1" s="67" t="n">
-        <v>44334.99849820978</v>
-      </c>
-      <c r="O1" s="59" t="n"/>
+      <c r="N1" s="80" t="n">
+        <v>44337.86379885743</v>
+      </c>
+      <c r="O1" s="57" t="n"/>
     </row>
     <row customHeight="1" ht="16.2" r="2" thickBot="1">
-      <c r="A2" s="68" t="inlineStr">
+      <c r="A2" s="61" t="inlineStr">
         <is>
           <t>Değerler</t>
         </is>
       </c>
-      <c r="B2" s="58" t="n"/>
-      <c r="C2" s="58" t="n"/>
-      <c r="D2" s="58" t="n"/>
-      <c r="E2" s="58" t="n"/>
-      <c r="F2" s="58" t="n"/>
-      <c r="G2" s="58" t="n"/>
-      <c r="H2" s="58" t="n"/>
-      <c r="I2" s="58" t="n"/>
-      <c r="J2" s="58" t="n"/>
-      <c r="K2" s="58" t="n"/>
-      <c r="L2" s="58" t="n"/>
-      <c r="M2" s="58" t="n"/>
-      <c r="N2" s="58" t="n"/>
-      <c r="O2" s="59" t="n"/>
+      <c r="B2" s="55" t="n"/>
+      <c r="C2" s="55" t="n"/>
+      <c r="D2" s="55" t="n"/>
+      <c r="E2" s="55" t="n"/>
+      <c r="F2" s="55" t="n"/>
+      <c r="G2" s="55" t="n"/>
+      <c r="H2" s="55" t="n"/>
+      <c r="I2" s="55" t="n"/>
+      <c r="J2" s="55" t="n"/>
+      <c r="K2" s="55" t="n"/>
+      <c r="L2" s="55" t="n"/>
+      <c r="M2" s="55" t="n"/>
+      <c r="N2" s="55" t="n"/>
+      <c r="O2" s="57" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
@@ -1301,40 +1310,40 @@
           <t>Güç :</t>
         </is>
       </c>
-      <c r="B3" s="60" t="inlineStr">
-        <is>
-          <t>62067.6 VA</t>
-        </is>
-      </c>
-      <c r="C3" s="80" t="n"/>
-      <c r="D3" s="80" t="n"/>
-      <c r="E3" s="80" t="n"/>
-      <c r="F3" s="62" t="n"/>
+      <c r="B3" s="81" t="inlineStr">
+        <is>
+          <t>18774.0 VA</t>
+        </is>
+      </c>
+      <c r="C3" s="82" t="n"/>
+      <c r="D3" s="82" t="n"/>
+      <c r="E3" s="82" t="n"/>
+      <c r="F3" s="60" t="n"/>
       <c r="G3" s="9" t="inlineStr">
         <is>
           <t>Primer Agirlik(Al) :</t>
         </is>
       </c>
-      <c r="H3" s="61" t="inlineStr">
-        <is>
-          <t>1.86 kg</t>
-        </is>
-      </c>
-      <c r="I3" s="62" t="n"/>
-      <c r="J3" s="81" t="inlineStr">
+      <c r="H3" s="83" t="inlineStr">
+        <is>
+          <t>1.772 kg</t>
+        </is>
+      </c>
+      <c r="I3" s="60" t="n"/>
+      <c r="J3" s="84" t="inlineStr">
         <is>
           <t xml:space="preserve">Karkas Ölçüleri : </t>
         </is>
       </c>
-      <c r="K3" s="70" t="n"/>
-      <c r="L3" s="82" t="inlineStr">
+      <c r="K3" s="63" t="n"/>
+      <c r="L3" s="85" t="inlineStr">
         <is>
           <t>50.0 x 100.0 x 143.0</t>
         </is>
       </c>
-      <c r="M3" s="69" t="n"/>
-      <c r="N3" s="69" t="n"/>
-      <c r="O3" s="70" t="n"/>
+      <c r="M3" s="62" t="n"/>
+      <c r="N3" s="62" t="n"/>
+      <c r="O3" s="63" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
@@ -1342,34 +1351,34 @@
           <t>Sac kk :</t>
         </is>
       </c>
-      <c r="B4" s="60" t="inlineStr">
+      <c r="B4" s="81" t="inlineStr">
         <is>
           <t>6.0</t>
         </is>
       </c>
-      <c r="C4" s="80" t="n"/>
-      <c r="D4" s="80" t="n"/>
-      <c r="E4" s="80" t="n"/>
-      <c r="F4" s="62" t="n"/>
+      <c r="C4" s="82" t="n"/>
+      <c r="D4" s="82" t="n"/>
+      <c r="E4" s="82" t="n"/>
+      <c r="F4" s="60" t="n"/>
       <c r="G4" s="9" t="inlineStr">
         <is>
           <t>Sekonder Agirlik(Al):</t>
         </is>
       </c>
-      <c r="H4" s="61" t="inlineStr"/>
-      <c r="I4" s="62" t="n"/>
-      <c r="J4" s="83" t="inlineStr">
+      <c r="H4" s="83" t="inlineStr"/>
+      <c r="I4" s="60" t="n"/>
+      <c r="J4" s="86" t="inlineStr">
         <is>
           <t xml:space="preserve">Trafo Ölçüleri : </t>
         </is>
       </c>
-      <c r="K4" s="84" t="n"/>
-      <c r="L4" s="85" t="inlineStr">
+      <c r="K4" s="87" t="n"/>
+      <c r="L4" s="88" t="inlineStr">
         <is>
           <t>0.0 x 0.0 x 0.0 x 0.0 x 0.0</t>
         </is>
       </c>
-      <c r="O4" s="84" t="n"/>
+      <c r="O4" s="87" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
@@ -1377,38 +1386,38 @@
           <t>Sac ©</t>
         </is>
       </c>
-      <c r="B5" s="60" t="inlineStr">
+      <c r="B5" s="81" t="inlineStr">
         <is>
           <t>0.35 mm</t>
         </is>
       </c>
-      <c r="C5" s="80" t="n"/>
-      <c r="D5" s="80" t="n"/>
-      <c r="E5" s="80" t="n"/>
-      <c r="F5" s="62" t="n"/>
+      <c r="C5" s="82" t="n"/>
+      <c r="D5" s="82" t="n"/>
+      <c r="E5" s="82" t="n"/>
+      <c r="F5" s="60" t="n"/>
       <c r="G5" s="9" t="inlineStr">
         <is>
           <t>Primer Agirlik(Cu) :</t>
         </is>
       </c>
-      <c r="H5" s="61" t="inlineStr">
+      <c r="H5" s="83" t="inlineStr">
         <is>
           <t>0.0 kg</t>
         </is>
       </c>
-      <c r="I5" s="62" t="n"/>
-      <c r="J5" s="83" t="inlineStr">
+      <c r="I5" s="60" t="n"/>
+      <c r="J5" s="86" t="inlineStr">
         <is>
           <t xml:space="preserve">Klemens &amp; Ayak : </t>
         </is>
       </c>
-      <c r="K5" s="84" t="n"/>
-      <c r="L5" s="85" t="inlineStr">
+      <c r="K5" s="87" t="n"/>
+      <c r="L5" s="88" t="inlineStr">
         <is>
           <t xml:space="preserve"> / 0.0 / 0.0 - </t>
         </is>
       </c>
-      <c r="O5" s="84" t="n"/>
+      <c r="O5" s="87" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
@@ -1416,34 +1425,34 @@
           <t>Gauss :</t>
         </is>
       </c>
-      <c r="B6" s="60" t="inlineStr">
+      <c r="B6" s="81" t="inlineStr">
         <is>
           <t>12000.0</t>
         </is>
       </c>
-      <c r="C6" s="80" t="n"/>
-      <c r="D6" s="80" t="n"/>
-      <c r="E6" s="80" t="n"/>
-      <c r="F6" s="62" t="n"/>
+      <c r="C6" s="82" t="n"/>
+      <c r="D6" s="82" t="n"/>
+      <c r="E6" s="82" t="n"/>
+      <c r="F6" s="60" t="n"/>
       <c r="G6" s="9" t="inlineStr">
         <is>
           <t>Sekonder Agirlik(Cu) :</t>
         </is>
       </c>
-      <c r="H6" s="61" t="inlineStr"/>
-      <c r="I6" s="62" t="n"/>
-      <c r="J6" s="83" t="inlineStr">
+      <c r="H6" s="83" t="inlineStr"/>
+      <c r="I6" s="60" t="n"/>
+      <c r="J6" s="86" t="inlineStr">
         <is>
           <t xml:space="preserve">Sac Agirlik : </t>
         </is>
       </c>
-      <c r="K6" s="84" t="n"/>
-      <c r="L6" s="85" t="inlineStr">
+      <c r="K6" s="87" t="n"/>
+      <c r="L6" s="88" t="inlineStr">
         <is>
           <t>36.6 kg(EI Sac)</t>
         </is>
       </c>
-      <c r="O6" s="84" t="n"/>
+      <c r="O6" s="87" t="n"/>
     </row>
     <row customHeight="1" ht="15" r="7" thickBot="1">
       <c r="A7" s="4" t="inlineStr">
@@ -1451,28 +1460,28 @@
           <t>Frekans :</t>
         </is>
       </c>
-      <c r="B7" s="60" t="inlineStr">
+      <c r="B7" s="81" t="inlineStr">
         <is>
           <t>90.0 Hz</t>
         </is>
       </c>
-      <c r="C7" s="80" t="n"/>
-      <c r="D7" s="80" t="n"/>
-      <c r="E7" s="80" t="n"/>
-      <c r="F7" s="62" t="n"/>
+      <c r="C7" s="82" t="n"/>
+      <c r="D7" s="82" t="n"/>
+      <c r="E7" s="82" t="n"/>
+      <c r="F7" s="60" t="n"/>
       <c r="G7" s="10" t="inlineStr">
         <is>
           <t>Toplam Agirlik :</t>
         </is>
       </c>
-      <c r="H7" s="61" t="inlineStr">
-        <is>
-          <t>Al:1.86 //  Cu:0.0kg</t>
-        </is>
-      </c>
-      <c r="I7" s="62" t="n"/>
-      <c r="J7" s="86" t="n"/>
-      <c r="K7" s="87" t="n"/>
+      <c r="H7" s="83" t="inlineStr">
+        <is>
+          <t>Al:1.772 //  Cu:0.0kg</t>
+        </is>
+      </c>
+      <c r="I7" s="60" t="n"/>
+      <c r="J7" s="89" t="n"/>
+      <c r="K7" s="90" t="n"/>
       <c r="L7" s="32" t="n"/>
       <c r="M7" s="31" t="n"/>
       <c r="N7" s="31" t="n"/>
@@ -1482,25 +1491,25 @@
       <c r="A8" s="1" t="n"/>
     </row>
     <row customHeight="1" ht="15" r="9" thickBot="1">
-      <c r="A9" s="57" t="inlineStr">
+      <c r="A9" s="76" t="inlineStr">
         <is>
           <t>Primer</t>
         </is>
       </c>
-      <c r="B9" s="58" t="n"/>
-      <c r="C9" s="58" t="n"/>
-      <c r="D9" s="58" t="n"/>
-      <c r="E9" s="58" t="n"/>
-      <c r="F9" s="58" t="n"/>
-      <c r="G9" s="59" t="n"/>
+      <c r="B9" s="55" t="n"/>
+      <c r="C9" s="55" t="n"/>
+      <c r="D9" s="55" t="n"/>
+      <c r="E9" s="55" t="n"/>
+      <c r="F9" s="55" t="n"/>
+      <c r="G9" s="57" t="n"/>
       <c r="I9" s="1" t="n"/>
       <c r="J9" s="1" t="n"/>
-      <c r="K9" s="88" t="inlineStr">
+      <c r="K9" s="91" t="inlineStr">
         <is>
           <t>Hesap Değerleri</t>
         </is>
       </c>
-      <c r="L9" s="70" t="n"/>
+      <c r="L9" s="63" t="n"/>
       <c r="M9" s="1" t="n"/>
       <c r="O9" s="1" t="n"/>
     </row>
@@ -1508,13 +1517,13 @@
       <c r="A10" s="1" t="n"/>
       <c r="G10" s="2" t="inlineStr">
         <is>
-          <t>1477.8 V ( 1477.8V )</t>
+          <t>447.0 V ( 447.0V )</t>
         </is>
       </c>
       <c r="I10" s="1" t="n"/>
       <c r="K10" s="46" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hava Aralığı </t>
+          <t>Boşluk</t>
         </is>
       </c>
       <c r="L10" s="50" t="n">
@@ -1523,7 +1532,7 @@
       <c r="O10" s="2" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="89" t="inlineStr">
+      <c r="A11" s="92" t="inlineStr">
         <is>
           <t>1 NOLU KADEME:</t>
         </is>
@@ -1534,13 +1543,13 @@
           <t>Endüktans(mH)</t>
         </is>
       </c>
-      <c r="L11" s="90" t="n">
-        <v>56</v>
+      <c r="L11" s="93" t="n">
+        <v>56.462</v>
       </c>
       <c r="M11" s="1" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="91" t="inlineStr">
+      <c r="A12" s="94" t="inlineStr">
         <is>
           <t>Tel :</t>
         </is>
@@ -1566,7 +1575,7 @@
       <c r="M12" s="22" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" s="91" t="inlineStr">
+      <c r="A13" s="94" t="inlineStr">
         <is>
           <t>Cap :</t>
         </is>
@@ -1590,7 +1599,7 @@
       <c r="M13" s="21" t="n"/>
     </row>
     <row r="14">
-      <c r="A14" s="91" t="inlineStr">
+      <c r="A14" s="94" t="inlineStr">
         <is>
           <t>Kesit :</t>
         </is>
@@ -1610,13 +1619,13 @@
         </is>
       </c>
       <c r="L14" s="51" t="n">
-        <v>9587.921</v>
+        <v>2900.122</v>
       </c>
       <c r="M14" s="21" t="n"/>
       <c r="O14" s="1" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="91" t="inlineStr">
+      <c r="A15" s="94" t="inlineStr">
         <is>
           <t>Akim :</t>
         </is>
@@ -1636,13 +1645,13 @@
         </is>
       </c>
       <c r="L15" s="51" t="n">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="M15" s="21" t="n"/>
       <c r="O15" s="2" t="n"/>
     </row>
     <row r="16">
-      <c r="A16" s="91" t="inlineStr">
+      <c r="A16" s="94" t="inlineStr">
         <is>
           <t>Kat :</t>
         </is>
@@ -1661,18 +1670,18 @@
         </is>
       </c>
       <c r="L16" s="51" t="n">
-        <v>90.97</v>
+        <v>50.03</v>
       </c>
       <c r="M16" s="21" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" s="91" t="inlineStr">
+      <c r="A17" s="94" t="inlineStr">
         <is>
           <t>Uzunluk :</t>
         </is>
       </c>
       <c r="B17" s="26" t="n">
-        <v>46.78593000000001</v>
+        <v>44.55411000000001</v>
       </c>
       <c r="C17" s="21" t="n"/>
       <c r="D17" s="21" t="n"/>
@@ -1690,8 +1699,8 @@
       <c r="M17" s="21" t="n"/>
     </row>
     <row r="18">
-      <c r="B18" s="92" t="inlineStr"/>
-      <c r="C18" s="91" t="inlineStr">
+      <c r="B18" s="95" t="inlineStr"/>
+      <c r="C18" s="94" t="inlineStr">
         <is>
           <t>-- Teller --</t>
         </is>
@@ -1706,18 +1715,18 @@
         </is>
       </c>
       <c r="L18" s="51" t="n">
-        <v>355.859</v>
+        <v>107.639</v>
       </c>
       <c r="M18" s="25" t="n"/>
       <c r="O18" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="15" r="19">
-      <c r="A19" s="91" t="inlineStr">
+      <c r="A19" s="94" t="inlineStr">
         <is>
           <t>Yuv. Tel :</t>
         </is>
       </c>
-      <c r="B19" s="93" t="n">
+      <c r="B19" s="96" t="n">
         <v>2.5</v>
       </c>
       <c r="C19" s="24" t="n"/>
@@ -1725,7 +1734,7 @@
       <c r="E19" s="24" t="n"/>
       <c r="G19" s="17" t="inlineStr">
         <is>
-          <t>135 sp</t>
+          <t>129 sp</t>
         </is>
       </c>
       <c r="I19" s="23" t="n"/>
@@ -1736,19 +1745,19 @@
         </is>
       </c>
       <c r="L19" s="51" t="n">
-        <v>1.421</v>
+        <v>0.129</v>
       </c>
       <c r="M19" s="24" t="n"/>
       <c r="O19" s="17" t="n"/>
     </row>
     <row customHeight="1" ht="15" r="20">
-      <c r="A20" s="91" t="inlineStr">
+      <c r="A20" s="94" t="inlineStr">
         <is>
           <t>Ytel Agr :</t>
         </is>
       </c>
-      <c r="B20" s="93" t="n">
-        <v>0.6200817214754518</v>
+      <c r="B20" s="96" t="n">
+        <v>0.5905020852980082</v>
       </c>
       <c r="C20" s="26" t="n"/>
       <c r="D20" s="26" t="n"/>
@@ -1761,12 +1770,12 @@
         </is>
       </c>
       <c r="L20" s="51" t="n">
-        <v>2.066</v>
+        <v>1.14</v>
       </c>
       <c r="M20" s="26" t="n"/>
     </row>
     <row customHeight="1" ht="15" r="21">
-      <c r="A21" s="91" t="inlineStr">
+      <c r="A21" s="94" t="inlineStr">
         <is>
           <t>Kare Tel :</t>
         </is>
@@ -1783,12 +1792,12 @@
         </is>
       </c>
       <c r="L21" s="51" t="n">
-        <v>247.583</v>
+        <v>100.792</v>
       </c>
       <c r="M21" s="24" t="n"/>
     </row>
     <row customHeight="1" ht="15" r="22">
-      <c r="A22" s="91" t="inlineStr">
+      <c r="A22" s="94" t="inlineStr">
         <is>
           <t>Ktel Agr :</t>
         </is>
@@ -1805,12 +1814,12 @@
         </is>
       </c>
       <c r="L22" s="51" t="n">
-        <v>1.29</v>
+        <v>0.02</v>
       </c>
       <c r="M22" s="26" t="n"/>
     </row>
     <row customHeight="1" ht="15" r="23">
-      <c r="A23" s="91" t="inlineStr">
+      <c r="A23" s="94" t="inlineStr">
         <is>
           <t>Folyo :</t>
         </is>
@@ -1827,12 +1836,12 @@
         </is>
       </c>
       <c r="L23" s="51" t="n">
-        <v>1.983</v>
+        <v>1.023</v>
       </c>
       <c r="M23" s="24" t="n"/>
     </row>
     <row customHeight="1" ht="15" r="24">
-      <c r="A24" s="91" t="inlineStr">
+      <c r="A24" s="94" t="inlineStr">
         <is>
           <t>Folyo Agr :</t>
         </is>
@@ -1849,12 +1858,12 @@
         </is>
       </c>
       <c r="L24" s="51" t="n">
-        <v>240.414</v>
+        <v>37.999</v>
       </c>
       <c r="M24" s="26" t="n"/>
     </row>
     <row customHeight="1" ht="15" r="25">
-      <c r="A25" s="91" t="inlineStr">
+      <c r="A25" s="94" t="inlineStr">
         <is>
           <t>Kapton :</t>
         </is>
@@ -1894,7 +1903,7 @@
         </is>
       </c>
       <c r="L27" s="52" t="n">
-        <v>135.097</v>
+        <v>128.724</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="28"/>
@@ -1916,14 +1925,14 @@
       <c r="G34" s="15" t="n"/>
     </row>
     <row customHeight="1" ht="15" r="35" thickBot="1">
-      <c r="B35" s="94" t="inlineStr">
+      <c r="B35" s="97" t="inlineStr">
         <is>
           <t>Primer Kademe</t>
         </is>
       </c>
-      <c r="C35" s="58" t="n"/>
-      <c r="D35" s="58" t="n"/>
-      <c r="E35" s="59" t="n"/>
+      <c r="C35" s="55" t="n"/>
+      <c r="D35" s="55" t="n"/>
+      <c r="E35" s="57" t="n"/>
       <c r="F35" s="7" t="inlineStr">
         <is>
           <t>Tur</t>
@@ -1936,14 +1945,14 @@
       </c>
     </row>
     <row customHeight="1" ht="15" r="36" thickBot="1">
-      <c r="B36" s="95" t="inlineStr">
+      <c r="B36" s="98" t="inlineStr">
         <is>
           <t>Yok</t>
         </is>
       </c>
-      <c r="C36" s="58" t="n"/>
-      <c r="D36" s="58" t="n"/>
-      <c r="E36" s="96" t="n"/>
+      <c r="C36" s="55" t="n"/>
+      <c r="D36" s="55" t="n"/>
+      <c r="E36" s="99" t="n"/>
       <c r="F36" s="18" t="inlineStr">
         <is>
           <t>Yok</t>
@@ -1956,14 +1965,14 @@
       </c>
     </row>
     <row customHeight="1" ht="15" r="37" thickBot="1">
-      <c r="B37" s="94" t="inlineStr">
+      <c r="B37" s="97" t="inlineStr">
         <is>
           <t xml:space="preserve">VA Kademe </t>
         </is>
       </c>
-      <c r="C37" s="58" t="n"/>
-      <c r="D37" s="58" t="n"/>
-      <c r="E37" s="59" t="n"/>
+      <c r="C37" s="55" t="n"/>
+      <c r="D37" s="55" t="n"/>
+      <c r="E37" s="57" t="n"/>
       <c r="F37" s="7" t="inlineStr">
         <is>
           <t>Tur</t>
@@ -1976,14 +1985,14 @@
       </c>
     </row>
     <row customHeight="1" ht="15" r="38" thickBot="1">
-      <c r="B38" s="95" t="inlineStr">
+      <c r="B38" s="98" t="inlineStr">
         <is>
           <t>Yok</t>
         </is>
       </c>
-      <c r="C38" s="58" t="n"/>
-      <c r="D38" s="58" t="n"/>
-      <c r="E38" s="96" t="n"/>
+      <c r="C38" s="55" t="n"/>
+      <c r="D38" s="55" t="n"/>
+      <c r="E38" s="99" t="n"/>
       <c r="F38" s="18" t="inlineStr">
         <is>
           <t>Yok</t>
@@ -1996,14 +2005,14 @@
       </c>
     </row>
     <row customHeight="1" ht="15" r="39" thickBot="1">
-      <c r="B39" s="94" t="inlineStr">
+      <c r="B39" s="97" t="inlineStr">
         <is>
           <t>Primer-Sekonder</t>
         </is>
       </c>
-      <c r="C39" s="58" t="n"/>
-      <c r="D39" s="58" t="n"/>
-      <c r="E39" s="59" t="n"/>
+      <c r="C39" s="55" t="n"/>
+      <c r="D39" s="55" t="n"/>
+      <c r="E39" s="57" t="n"/>
       <c r="F39" s="7" t="inlineStr">
         <is>
           <t>Tur</t>
@@ -2012,14 +2021,14 @@
       <c r="G39" s="8" t="n"/>
     </row>
     <row customHeight="1" ht="15" r="40" thickBot="1">
-      <c r="B40" s="95" t="inlineStr">
+      <c r="B40" s="98" t="inlineStr">
         <is>
           <t>Yok</t>
         </is>
       </c>
-      <c r="C40" s="58" t="n"/>
-      <c r="D40" s="58" t="n"/>
-      <c r="E40" s="96" t="n"/>
+      <c r="C40" s="55" t="n"/>
+      <c r="D40" s="55" t="n"/>
+      <c r="E40" s="99" t="n"/>
       <c r="F40" s="20" t="inlineStr">
         <is>
           <t>Yok</t>
@@ -2169,6 +2178,14 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="K9:L9"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="B3:F3"/>
@@ -2185,14 +2202,6 @@
     <mergeCell ref="L5:O5"/>
     <mergeCell ref="L6:O6"/>
     <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="A9:G9"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="K9:L9"/>
     <mergeCell ref="B35:E35"/>
     <mergeCell ref="B36:E36"/>
     <mergeCell ref="B37:E37"/>
@@ -2235,10 +2244,10 @@
           <t>Malzeme Listesi</t>
         </is>
       </c>
-      <c r="C1" s="97" t="n"/>
-      <c r="D1" s="97" t="n"/>
-      <c r="E1" s="97" t="n"/>
-      <c r="F1" s="98" t="n"/>
+      <c r="C1" s="100" t="n"/>
+      <c r="D1" s="100" t="n"/>
+      <c r="E1" s="100" t="n"/>
+      <c r="F1" s="101" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="42" t="n"/>
@@ -2275,7 +2284,7 @@
         </is>
       </c>
       <c r="D3" s="45" t="n">
-        <v>0.6200817214754518</v>
+        <v>0.5905020852980082</v>
       </c>
       <c r="E3" s="42" t="n"/>
       <c r="F3" s="42" t="n"/>

</xml_diff>